<commit_message>
Revision of everything in the document
</commit_message>
<xml_diff>
--- a/FEAT - UC.xlsx
+++ b/FEAT - UC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Feature 1</t>
   </si>
@@ -177,7 +177,13 @@
     <t>Project Name: Self Start Assignment Two</t>
   </si>
   <si>
-    <t>Use Cases-to-Entity Class Traceability Matrix</t>
+    <t>X represents a relationship</t>
+  </si>
+  <si>
+    <t>Represents that it is not directly related to any use case</t>
+  </si>
+  <si>
+    <t>Use Cases-to-Feature Class Traceability Matrix</t>
   </si>
 </sst>
 </file>
@@ -320,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,6 +363,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,15 +387,585 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -428,585 +1005,15 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
+        <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -1023,28 +1030,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G6:Y36" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G6:Y36" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="G6:Y36"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="Features/ Use Cases" dataDxfId="18"/>
-    <tableColumn id="2" name="ManageDynamicForms" dataDxfId="17"/>
+    <tableColumn id="1" name="Features/ Use Cases" dataDxfId="16"/>
+    <tableColumn id="2" name="ManageDynamicForms" dataDxfId="15"/>
     <tableColumn id="3" name="ManageAccounts"/>
-    <tableColumn id="4" name="ManageExercise" dataDxfId="16"/>
-    <tableColumn id="5" name="ManageRehabPlans" dataDxfId="15"/>
-    <tableColumn id="6" name="ManageAssessmentTests" dataDxfId="14"/>
-    <tableColumn id="7" name="AssignExercises/Tests" dataDxfId="13"/>
-    <tableColumn id="8" name="AssignPlans" dataDxfId="12"/>
-    <tableColumn id="9" name="GenerateAssessmentReport" dataDxfId="11"/>
-    <tableColumn id="10" name="ManageTreatment" dataDxfId="10"/>
-    <tableColumn id="11" name="ManageRubrics" dataDxfId="9"/>
-    <tableColumn id="12" name="DisplayUserHistory" dataDxfId="8"/>
-    <tableColumn id="13" name="ChangePassword" dataDxfId="7"/>
-    <tableColumn id="14" name="CreateAccount" dataDxfId="6"/>
-    <tableColumn id="15" name="SubmitInjuryForm" dataDxfId="5"/>
-    <tableColumn id="16" name="CompleteAssessmentTest" dataDxfId="4"/>
+    <tableColumn id="4" name="ManageExercise" dataDxfId="14"/>
+    <tableColumn id="5" name="ManageRehabPlans" dataDxfId="13"/>
+    <tableColumn id="6" name="ManageAssessmentTests" dataDxfId="12"/>
+    <tableColumn id="7" name="AssignExercises/Tests" dataDxfId="11"/>
+    <tableColumn id="8" name="AssignPlans" dataDxfId="10"/>
+    <tableColumn id="9" name="GenerateAssessmentReport" dataDxfId="9"/>
+    <tableColumn id="10" name="ManageTreatment" dataDxfId="8"/>
+    <tableColumn id="11" name="ManageRubrics" dataDxfId="7"/>
+    <tableColumn id="12" name="DisplayUserHistory" dataDxfId="6"/>
+    <tableColumn id="13" name="ChangePassword" dataDxfId="5"/>
+    <tableColumn id="14" name="CreateAccount" dataDxfId="4"/>
+    <tableColumn id="15" name="SubmitInjuryForm" dataDxfId="3"/>
+    <tableColumn id="16" name="CompleteAssessmentTest" dataDxfId="2"/>
     <tableColumn id="17" name="MakePayment"/>
-    <tableColumn id="18" name="ManageAppointments" dataDxfId="3"/>
-    <tableColumn id="19" name="View/PerformTreatmentPlans" dataDxfId="2"/>
+    <tableColumn id="18" name="ManageAppointments" dataDxfId="1"/>
+    <tableColumn id="19" name="View/PerformTreatmentPlans" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1315,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1328,7 +1335,8 @@
     <col min="6" max="6" width="16.47265625" customWidth="1"/>
     <col min="7" max="7" width="30.3671875" customWidth="1"/>
     <col min="8" max="8" width="36.9453125" customWidth="1"/>
-    <col min="9" max="10" width="24" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="45.7890625" customWidth="1"/>
     <col min="11" max="11" width="29.62890625" customWidth="1"/>
     <col min="12" max="12" width="32.26171875" customWidth="1"/>
     <col min="13" max="13" width="31.62890625" customWidth="1"/>
@@ -1366,10 +1374,18 @@
         <v>51</v>
       </c>
     </row>
+    <row r="3" spans="6:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="4" spans="6:25" ht="18.3" x14ac:dyDescent="0.7">
       <c r="G4" s="3"/>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="6:25" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">

</xml_diff>